<commit_message>
Add new Excel files for used and valid unique SMILES
</commit_message>
<xml_diff>
--- a/Used_SMILES.xlsx
+++ b/Used_SMILES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46A121EE-555B-4213-B035-072B1C02FF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E4DF31-4375-471D-A18D-D7C4E79F1531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Till Now</t>
   </si>
@@ -51,9 +51,6 @@
     <t>M20</t>
   </si>
   <si>
-    <t>M7</t>
-  </si>
-  <si>
     <t>M15(Si)</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>M25(Cy)</t>
   </si>
   <si>
-    <t>M261(Hetro)</t>
-  </si>
-  <si>
     <t>M4</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>M28(Cy)</t>
   </si>
   <si>
-    <t>M663(Hetro)</t>
-  </si>
-  <si>
     <t>M45</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>M49(Cy)</t>
   </si>
   <si>
-    <t>M687(Hetro)</t>
-  </si>
-  <si>
     <t>M56</t>
   </si>
   <si>
@@ -162,9 +150,6 @@
     <t>M57(Cy)</t>
   </si>
   <si>
-    <t>M919(Hetro)</t>
-  </si>
-  <si>
     <t>M68</t>
   </si>
   <si>
@@ -192,9 +177,6 @@
     <t>M71(Cy)</t>
   </si>
   <si>
-    <t>M1107(Hetro)</t>
-  </si>
-  <si>
     <t>M70</t>
   </si>
   <si>
@@ -222,9 +204,6 @@
     <t>M78(Cy)</t>
   </si>
   <si>
-    <t>M2111(Hetro)</t>
-  </si>
-  <si>
     <t>M96</t>
   </si>
   <si>
@@ -340,6 +319,273 @@
   </si>
   <si>
     <t>M2815</t>
+  </si>
+  <si>
+    <t>M261(Charged_Hetro)</t>
+  </si>
+  <si>
+    <t>M663(Charged_Hetro)</t>
+  </si>
+  <si>
+    <t>M687(Charged_Hetro)</t>
+  </si>
+  <si>
+    <t>M919(Charged_Hetro)</t>
+  </si>
+  <si>
+    <t>M1107(Charged_Hetro)</t>
+  </si>
+  <si>
+    <t>M2111(Charged_Hetro)</t>
+  </si>
+  <si>
+    <t>M77(Hetro)</t>
+  </si>
+  <si>
+    <t>M79(Hetro)</t>
+  </si>
+  <si>
+    <t>M134(Hetro)</t>
+  </si>
+  <si>
+    <t>M155(Hetro)</t>
+  </si>
+  <si>
+    <t>M178(Hetro)</t>
+  </si>
+  <si>
+    <t>M200(Hetro)</t>
+  </si>
+  <si>
+    <t>M315(Hetro)</t>
+  </si>
+  <si>
+    <t>M8(Benz)</t>
+  </si>
+  <si>
+    <t>M10(Benz)</t>
+  </si>
+  <si>
+    <t>M14(Benz)</t>
+  </si>
+  <si>
+    <t>M21(Benz)</t>
+  </si>
+  <si>
+    <t>M66(Benz)</t>
+  </si>
+  <si>
+    <t>M107(Benz</t>
+  </si>
+  <si>
+    <t>M109(Benz)</t>
+  </si>
+  <si>
+    <t>M211(polar)</t>
+  </si>
+  <si>
+    <t>M279(Polar)</t>
+  </si>
+  <si>
+    <t>M283(Polar)</t>
+  </si>
+  <si>
+    <t>M314(Polar)</t>
+  </si>
+  <si>
+    <t>M322(Polar)</t>
+  </si>
+  <si>
+    <t>M337(Polar)</t>
+  </si>
+  <si>
+    <t>M357(Polar)</t>
+  </si>
+  <si>
+    <t>M372(Polar)</t>
+  </si>
+  <si>
+    <t>M427(Polar)</t>
+  </si>
+  <si>
+    <t>Polar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicon </t>
+  </si>
+  <si>
+    <t>M100</t>
+  </si>
+  <si>
+    <t>M110</t>
+  </si>
+  <si>
+    <t>M121</t>
+  </si>
+  <si>
+    <t>M122</t>
+  </si>
+  <si>
+    <t>M133</t>
+  </si>
+  <si>
+    <t>M157</t>
+  </si>
+  <si>
+    <t>M7(Polar)</t>
+  </si>
+  <si>
+    <t>M191</t>
+  </si>
+  <si>
+    <t>M232</t>
+  </si>
+  <si>
+    <t>M111</t>
+  </si>
+  <si>
+    <t>M181</t>
+  </si>
+  <si>
+    <t>M212</t>
+  </si>
+  <si>
+    <t>M229</t>
+  </si>
+  <si>
+    <t>M241</t>
+  </si>
+  <si>
+    <t>M509</t>
+  </si>
+  <si>
+    <t>Tert-Butyl</t>
+  </si>
+  <si>
+    <t>M105</t>
+  </si>
+  <si>
+    <t>M106</t>
+  </si>
+  <si>
+    <t>M114</t>
+  </si>
+  <si>
+    <t>M117</t>
+  </si>
+  <si>
+    <t>M130</t>
+  </si>
+  <si>
+    <t>M132</t>
+  </si>
+  <si>
+    <t>M139</t>
+  </si>
+  <si>
+    <t>M149</t>
+  </si>
+  <si>
+    <t>M152</t>
+  </si>
+  <si>
+    <t>M158</t>
+  </si>
+  <si>
+    <t>Chlorine Cl</t>
+  </si>
+  <si>
+    <t>M177</t>
+  </si>
+  <si>
+    <t>M189</t>
+  </si>
+  <si>
+    <t>M201</t>
+  </si>
+  <si>
+    <t>M205</t>
+  </si>
+  <si>
+    <t>M218</t>
+  </si>
+  <si>
+    <t>M251</t>
+  </si>
+  <si>
+    <t>M258</t>
+  </si>
+  <si>
+    <t>M304</t>
+  </si>
+  <si>
+    <t>M326</t>
+  </si>
+  <si>
+    <t>Ketone</t>
+  </si>
+  <si>
+    <t>M80</t>
+  </si>
+  <si>
+    <t>M113</t>
+  </si>
+  <si>
+    <t>M116</t>
+  </si>
+  <si>
+    <t>M126</t>
+  </si>
+  <si>
+    <t>M137</t>
+  </si>
+  <si>
+    <t>M164</t>
+  </si>
+  <si>
+    <t>M165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulfone </t>
+  </si>
+  <si>
+    <t>M296</t>
+  </si>
+  <si>
+    <t>M342</t>
+  </si>
+  <si>
+    <t>M359</t>
+  </si>
+  <si>
+    <t>M437</t>
+  </si>
+  <si>
+    <t>M441</t>
+  </si>
+  <si>
+    <t>M519</t>
+  </si>
+  <si>
+    <t>M581</t>
+  </si>
+  <si>
+    <t>M692</t>
+  </si>
+  <si>
+    <t>M748</t>
+  </si>
+  <si>
+    <t>M848</t>
+  </si>
+  <si>
+    <t>Cyano C#N</t>
+  </si>
+  <si>
+    <t>M123</t>
+  </si>
+  <si>
+    <t>M156</t>
   </si>
 </sst>
 </file>
@@ -355,7 +601,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +626,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -469,15 +727,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,40 +861,70 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -843,413 +1241,621 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE12E00B-2345-41BD-89EE-DDF317AEFD3A}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J39"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="55" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4">
-        <v>45691</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11">
+        <v>45692</v>
+      </c>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="11">
+        <v>45934</v>
+      </c>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="J3" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="F4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="H4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="I4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="J4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="D5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="F5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="G5" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="H5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="I5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="11" t="s">
+      <c r="J5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="D6" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="F6" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="G6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="H6" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="I6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="J6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="N6" s="14"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="D7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="F7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="G7" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="H7" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="I7" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="J7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="D8" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="E8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="F8" s="25" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="G8" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="H8" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="I8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="J8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="28">
+        <v>45965</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="H10" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17" t="s">
+      <c r="C11" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="C12" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>173</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>174</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>175</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>78</v>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="C15" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>176</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>79</v>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="C16" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>177</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>80</v>
+      <c r="A17" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="C17" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>178</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>81</v>
+      <c r="A18" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="C18" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>179</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>82</v>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="C19" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>83</v>
+    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1262,8 +1868,8 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>84</v>
+      <c r="A21" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1276,8 +1882,8 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>85</v>
+      <c r="A22" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1290,8 +1896,8 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>86</v>
+      <c r="A23" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1304,8 +1910,8 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>87</v>
+      <c r="A24" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1318,8 +1924,8 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>88</v>
+      <c r="A25" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1332,8 +1938,8 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>89</v>
+      <c r="A26" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1346,8 +1952,8 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>90</v>
+      <c r="A27" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1360,8 +1966,8 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>91</v>
+      <c r="A28" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1374,8 +1980,8 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>92</v>
+      <c r="A29" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1388,8 +1994,8 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>92</v>
+      <c r="A30" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1402,8 +2008,8 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>93</v>
+      <c r="A31" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1416,8 +2022,8 @@
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>94</v>
+      <c r="A32" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1430,8 +2036,8 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>95</v>
+      <c r="A33" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1444,8 +2050,8 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>96</v>
+      <c r="A34" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1458,11 +2064,10 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>97</v>
+      <c r="A35" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1472,11 +2077,10 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>98</v>
+      <c r="A36" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1486,8 +2090,8 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>99</v>
+      <c r="A37" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B37" s="1"/>
       <c r="D37" s="1"/>
@@ -1499,8 +2103,8 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>100</v>
+      <c r="A38" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B38" s="1"/>
       <c r="D38" s="1"/>
@@ -1511,24 +2115,14 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="C9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new Excel files for used and valid unique SMILES data
</commit_message>
<xml_diff>
--- a/Used_SMILES.xlsx
+++ b/Used_SMILES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B0DDD5-8655-4CD9-9B76-82DF75D11858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C931B2-A04B-45BF-A3A1-D0FB99DCF2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="272">
   <si>
     <t>Till Now</t>
   </si>
@@ -579,13 +579,277 @@
     <t>M848</t>
   </si>
   <si>
-    <t>Cyano C#N</t>
-  </si>
-  <si>
     <t>M123</t>
   </si>
   <si>
     <t>M156</t>
+  </si>
+  <si>
+    <t>M185</t>
+  </si>
+  <si>
+    <t>22/04/2025</t>
+  </si>
+  <si>
+    <t>M187</t>
+  </si>
+  <si>
+    <t>M195</t>
+  </si>
+  <si>
+    <t>M209</t>
+  </si>
+  <si>
+    <t>M214</t>
+  </si>
+  <si>
+    <t>M237</t>
+  </si>
+  <si>
+    <t>M245</t>
+  </si>
+  <si>
+    <t>M253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyano </t>
+  </si>
+  <si>
+    <t>Charged Hetro</t>
+  </si>
+  <si>
+    <t>M2166</t>
+  </si>
+  <si>
+    <t>M2650</t>
+  </si>
+  <si>
+    <t>M2652</t>
+  </si>
+  <si>
+    <t>M2854</t>
+  </si>
+  <si>
+    <t>M336</t>
+  </si>
+  <si>
+    <t>M417</t>
+  </si>
+  <si>
+    <t>M429</t>
+  </si>
+  <si>
+    <t>M455</t>
+  </si>
+  <si>
+    <t>M468</t>
+  </si>
+  <si>
+    <t>M499</t>
+  </si>
+  <si>
+    <t>M510</t>
+  </si>
+  <si>
+    <t>M626</t>
+  </si>
+  <si>
+    <t>M704</t>
+  </si>
+  <si>
+    <t>M176</t>
+  </si>
+  <si>
+    <t>M208</t>
+  </si>
+  <si>
+    <t>M217</t>
+  </si>
+  <si>
+    <t>M248</t>
+  </si>
+  <si>
+    <t>M252</t>
+  </si>
+  <si>
+    <t>Hetrocyclic Rings</t>
+  </si>
+  <si>
+    <t>Benzene</t>
+  </si>
+  <si>
+    <t>M255</t>
+  </si>
+  <si>
+    <t>M263</t>
+  </si>
+  <si>
+    <t>M298</t>
+  </si>
+  <si>
+    <t>M301</t>
+  </si>
+  <si>
+    <t>M596</t>
+  </si>
+  <si>
+    <t>M610</t>
+  </si>
+  <si>
+    <t>M611</t>
+  </si>
+  <si>
+    <t>M680</t>
+  </si>
+  <si>
+    <t>M694</t>
+  </si>
+  <si>
+    <t>M719</t>
+  </si>
+  <si>
+    <t>M826</t>
+  </si>
+  <si>
+    <t>M830</t>
+  </si>
+  <si>
+    <t>M274</t>
+  </si>
+  <si>
+    <t>M281</t>
+  </si>
+  <si>
+    <t>M285</t>
+  </si>
+  <si>
+    <t>M297</t>
+  </si>
+  <si>
+    <t>M160</t>
+  </si>
+  <si>
+    <t>M166</t>
+  </si>
+  <si>
+    <t>M180</t>
+  </si>
+  <si>
+    <t>M227</t>
+  </si>
+  <si>
+    <t>M346</t>
+  </si>
+  <si>
+    <t>M3454</t>
+  </si>
+  <si>
+    <t>M366</t>
+  </si>
+  <si>
+    <t>M367</t>
+  </si>
+  <si>
+    <t>M186</t>
+  </si>
+  <si>
+    <t>M216</t>
+  </si>
+  <si>
+    <t>M223</t>
+  </si>
+  <si>
+    <t>M238</t>
+  </si>
+  <si>
+    <t>23/04/2025</t>
+  </si>
+  <si>
+    <t>M890</t>
+  </si>
+  <si>
+    <t>M945</t>
+  </si>
+  <si>
+    <t>M952</t>
+  </si>
+  <si>
+    <t>M956</t>
+  </si>
+  <si>
+    <t>M276</t>
+  </si>
+  <si>
+    <t>M284</t>
+  </si>
+  <si>
+    <t>M286</t>
+  </si>
+  <si>
+    <t>M300</t>
+  </si>
+  <si>
+    <t>M751</t>
+  </si>
+  <si>
+    <t>M774</t>
+  </si>
+  <si>
+    <t>M807</t>
+  </si>
+  <si>
+    <t>M1001</t>
+  </si>
+  <si>
+    <t>M302</t>
+  </si>
+  <si>
+    <t>M320</t>
+  </si>
+  <si>
+    <t>M341</t>
+  </si>
+  <si>
+    <t>M364</t>
+  </si>
+  <si>
+    <t>M834</t>
+  </si>
+  <si>
+    <t>M894</t>
+  </si>
+  <si>
+    <t>M906</t>
+  </si>
+  <si>
+    <t>M935</t>
+  </si>
+  <si>
+    <t>M944</t>
+  </si>
+  <si>
+    <t>M949</t>
+  </si>
+  <si>
+    <t>M299</t>
+  </si>
+  <si>
+    <t>M311</t>
+  </si>
+  <si>
+    <t>M328</t>
+  </si>
+  <si>
+    <t>M335</t>
+  </si>
+  <si>
+    <t>M373</t>
+  </si>
+  <si>
+    <t>M407</t>
+  </si>
+  <si>
+    <t>M444</t>
   </si>
 </sst>
 </file>
@@ -601,7 +865,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,8 +902,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -697,17 +973,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -820,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,100 +1093,136 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1238,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE12E00B-2345-41BD-89EE-DDF317AEFD3A}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="55" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="85" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,74 +1554,81 @@
     <col min="6" max="6" width="12.88671875" customWidth="1"/>
     <col min="8" max="8" width="15.21875" customWidth="1"/>
     <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="10" max="10" width="22.21875" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="24.77734375" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="30">
         <v>45692</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="31">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="37">
         <v>45934</v>
       </c>
-      <c r="L1" s="33"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K1" s="38"/>
+      <c r="L1" s="28">
+        <v>45692</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="I2" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -1329,196 +1637,196 @@
       <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L5" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -1527,553 +1835,745 @@
       <c r="E8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="30">
         <v>45965</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="7" t="s">
+      <c r="I10" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="K10" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I12" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I13" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I14" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I15" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="L15" s="27"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I16" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I17" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="7"/>
+      <c r="C20" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="27"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="7"/>
+      <c r="C21" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="I21" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="J21" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="K21" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="L21" s="27"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="7"/>
+      <c r="C22" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I22" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="J22" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="K22" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="L22" s="27"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="I23" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="J23" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="K23" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="L23" s="27"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="7"/>
+      <c r="C24" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>246</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>254</v>
+      </c>
+      <c r="K24" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="L24" s="27"/>
+    </row>
+    <row r="25" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D25" s="4"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="C26" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="C28" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="C29" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="45" t="s">
+        <v>262</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="45" t="s">
+        <v>263</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="46" t="s">
+        <v>264</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>92</v>
       </c>
@@ -2084,9 +2584,8 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>93</v>
       </c>
@@ -2097,9 +2596,8 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>94</v>
       </c>
@@ -2110,14 +2608,16 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update binary files for SMILES datasets
</commit_message>
<xml_diff>
--- a/Used_SMILES.xlsx
+++ b/Used_SMILES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C931B2-A04B-45BF-A3A1-D0FB99DCF2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF20D638-EEA0-4A25-BF48-D178E8400538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="323">
   <si>
     <t>Till Now</t>
   </si>
@@ -850,6 +850,159 @@
   </si>
   <si>
     <t>M444</t>
+  </si>
+  <si>
+    <t>M466</t>
+  </si>
+  <si>
+    <t>M484</t>
+  </si>
+  <si>
+    <t>M488</t>
+  </si>
+  <si>
+    <t>28/04/2025</t>
+  </si>
+  <si>
+    <t>M231</t>
+  </si>
+  <si>
+    <t>M240</t>
+  </si>
+  <si>
+    <t>M243</t>
+  </si>
+  <si>
+    <t>M259</t>
+  </si>
+  <si>
+    <t>M260</t>
+  </si>
+  <si>
+    <t>M266</t>
+  </si>
+  <si>
+    <t>M287</t>
+  </si>
+  <si>
+    <t>M291</t>
+  </si>
+  <si>
+    <t>M293</t>
+  </si>
+  <si>
+    <t>M323</t>
+  </si>
+  <si>
+    <t>M378</t>
+  </si>
+  <si>
+    <t>M399</t>
+  </si>
+  <si>
+    <t>M439</t>
+  </si>
+  <si>
+    <t>M449</t>
+  </si>
+  <si>
+    <t>M459</t>
+  </si>
+  <si>
+    <t>M470</t>
+  </si>
+  <si>
+    <t>M500</t>
+  </si>
+  <si>
+    <t>M502</t>
+  </si>
+  <si>
+    <t>M511</t>
+  </si>
+  <si>
+    <t>M522</t>
+  </si>
+  <si>
+    <t>M239</t>
+  </si>
+  <si>
+    <t>M269</t>
+  </si>
+  <si>
+    <t>M247</t>
+  </si>
+  <si>
+    <t>M249</t>
+  </si>
+  <si>
+    <t>M262</t>
+  </si>
+  <si>
+    <t>M288</t>
+  </si>
+  <si>
+    <t>M333</t>
+  </si>
+  <si>
+    <t>M349</t>
+  </si>
+  <si>
+    <t>M353</t>
+  </si>
+  <si>
+    <t>M355</t>
+  </si>
+  <si>
+    <t>M1048</t>
+  </si>
+  <si>
+    <t>M1122</t>
+  </si>
+  <si>
+    <t>M1159</t>
+  </si>
+  <si>
+    <t>M1179</t>
+  </si>
+  <si>
+    <t>M1251</t>
+  </si>
+  <si>
+    <t>M1196</t>
+  </si>
+  <si>
+    <t>M1222</t>
+  </si>
+  <si>
+    <t>M1298</t>
+  </si>
+  <si>
+    <t>M1370</t>
+  </si>
+  <si>
+    <t>M1415</t>
+  </si>
+  <si>
+    <t>M306</t>
+  </si>
+  <si>
+    <t>M307</t>
+  </si>
+  <si>
+    <t>M313</t>
+  </si>
+  <si>
+    <t>M316</t>
+  </si>
+  <si>
+    <t>M321</t>
+  </si>
+  <si>
+    <t>M330</t>
+  </si>
+  <si>
+    <t>M358</t>
   </si>
 </sst>
 </file>
@@ -865,7 +1018,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -911,6 +1064,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1085,7 +1244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1096,9 +1255,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1174,39 +1330,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1223,6 +1346,66 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1541,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE12E00B-2345-41BD-89EE-DDF317AEFD3A}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="85" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="68" zoomScaleNormal="85" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,6 +1735,7 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="15.21875" customWidth="1"/>
     <col min="9" max="9" width="13.88671875" customWidth="1"/>
     <col min="10" max="10" width="20.44140625" customWidth="1"/>
@@ -1567,22 +1751,22 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="30">
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="35">
         <v>45692</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="37">
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="39">
         <v>45934</v>
       </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="28">
+      <c r="K1" s="40"/>
+      <c r="L1" s="27">
         <v>45692</v>
       </c>
     </row>
@@ -1593,34 +1777,34 @@
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>193</v>
       </c>
     </row>
@@ -1631,34 +1815,34 @@
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>95</v>
       </c>
       <c r="M3" s="1"/>
@@ -1670,34 +1854,34 @@
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>96</v>
       </c>
       <c r="M4" s="1"/>
@@ -1709,34 +1893,34 @@
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>97</v>
       </c>
       <c r="M5" s="1"/>
@@ -1748,34 +1932,34 @@
       <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>98</v>
       </c>
       <c r="M6" s="1"/>
@@ -1787,34 +1971,34 @@
       <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="11" t="s">
         <v>99</v>
       </c>
       <c r="M7" s="1"/>
@@ -1826,34 +2010,34 @@
       <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="11" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="1"/>
@@ -1865,20 +2049,20 @@
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="35">
         <v>45965</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1887,34 +2071,34 @@
       <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>194</v>
       </c>
     </row>
@@ -1925,34 +2109,34 @@
       <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>195</v>
       </c>
     </row>
@@ -1963,34 +2147,34 @@
       <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2001,34 +2185,34 @@
       <c r="B13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="5" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2039,538 +2223,640 @@
       <c r="B14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="L14" s="27"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="L15" s="27"/>
+      <c r="L15" s="26"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="L16" s="27"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="L17" s="27"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="L18" s="27"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="L19" s="27"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="32" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="32" t="s">
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="27"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H21" s="41" t="s">
+      <c r="H21" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="29" t="s">
         <v>247</v>
       </c>
-      <c r="J21" s="41" t="s">
+      <c r="J21" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="K21" s="42" t="s">
+      <c r="K21" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="L21" s="27"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="I22" s="41" t="s">
+      <c r="I22" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="K22" s="42" t="s">
+      <c r="K22" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="L22" s="27"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="5" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I23" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="J23" s="41" t="s">
+      <c r="J23" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="K23" s="42" t="s">
+      <c r="K23" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="L23" s="27"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="6"/>
+      <c r="C24" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="H24" s="43" t="s">
+      <c r="H24" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="I24" s="43" t="s">
+      <c r="I24" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="J24" s="43" t="s">
+      <c r="J24" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="K24" s="44" t="s">
+      <c r="K24" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="L24" s="27"/>
-    </row>
-    <row r="25" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="26"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="46" t="s">
+        <v>275</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="E26" s="49" t="s">
+        <v>276</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G26" s="49" t="s">
+        <v>296</v>
+      </c>
+      <c r="H26" s="52" t="s">
+        <v>306</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="E27" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="F27" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="G27" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="H27" s="53" t="s">
+        <v>307</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="E28" s="50" t="s">
+        <v>278</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="G28" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="H28" s="53" t="s">
+        <v>308</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="E29" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="F29" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="G29" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="H29" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="45" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="E30" s="50" t="s">
+        <v>280</v>
+      </c>
+      <c r="F30" s="50" t="s">
+        <v>290</v>
+      </c>
+      <c r="G30" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="H30" s="53" t="s">
+        <v>310</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="45" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="E31" s="50" t="s">
+        <v>281</v>
+      </c>
+      <c r="F31" s="50" t="s">
+        <v>291</v>
+      </c>
+      <c r="G31" s="50" t="s">
+        <v>301</v>
+      </c>
+      <c r="H31" s="53" t="s">
+        <v>311</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="45" t="s">
+      <c r="B32" s="6"/>
+      <c r="C32" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="E32" s="50" t="s">
+        <v>282</v>
+      </c>
+      <c r="F32" s="50" t="s">
+        <v>292</v>
+      </c>
+      <c r="G32" s="50" t="s">
+        <v>302</v>
+      </c>
+      <c r="H32" s="53" t="s">
+        <v>312</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="45" t="s">
+      <c r="B33" s="6"/>
+      <c r="C33" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="D33" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" s="50" t="s">
+        <v>283</v>
+      </c>
+      <c r="F33" s="50" t="s">
+        <v>293</v>
+      </c>
+      <c r="G33" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="H33" s="53" t="s">
+        <v>313</v>
+      </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="45" t="s">
+      <c r="B34" s="6"/>
+      <c r="C34" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="D34" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="E34" s="50" t="s">
+        <v>284</v>
+      </c>
+      <c r="F34" s="50" t="s">
+        <v>294</v>
+      </c>
+      <c r="G34" s="50" t="s">
+        <v>304</v>
+      </c>
+      <c r="H34" s="53" t="s">
+        <v>314</v>
+      </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="46" t="s">
+      <c r="B35" s="6"/>
+      <c r="C35" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="D35" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="E35" s="51" t="s">
+        <v>285</v>
+      </c>
+      <c r="F35" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="G35" s="51" t="s">
+        <v>305</v>
+      </c>
+      <c r="H35" s="54" t="s">
+        <v>315</v>
+      </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -2610,14 +2896,15 @@
       <c r="I38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement SMILES enumeration and validation in parallel using RDKit and multiprocessing
- Added a new script `smile_enum.py` for generating random SMILES strings from input SMILES.
- Integrated pandas for CSV handling and tqdm for progress tracking.
- Configured command-line arguments for input/output file names, enumeration count, and number of worker processes.
- Implemented error handling for invalid SMILES and file operations.
- Enhanced performance by utilizing multiprocessing for parallel enumeration.
- Included validation of generated SMILES to ensure structural integrity before saving to output CSV.
</commit_message>
<xml_diff>
--- a/Used_SMILES.xlsx
+++ b/Used_SMILES.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF20D638-EEA0-4A25-BF48-D178E8400538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B684897-BC69-42FC-9451-8611E335E259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Leemol" sheetId="1" r:id="rId1"/>
+    <sheet name="Christina Maam" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="330">
   <si>
     <t>Till Now</t>
   </si>
@@ -1003,6 +1004,27 @@
   </si>
   <si>
     <t>M358</t>
+  </si>
+  <si>
+    <t>M406</t>
+  </si>
+  <si>
+    <t>M457</t>
+  </si>
+  <si>
+    <t>M411</t>
+  </si>
+  <si>
+    <t>M516</t>
+  </si>
+  <si>
+    <t>M520</t>
+  </si>
+  <si>
+    <t>M521</t>
+  </si>
+  <si>
+    <t>M635</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1348,64 +1370,67 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1724,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE12E00B-2345-41BD-89EE-DDF317AEFD3A}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="68" zoomScaleNormal="85" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="F18" zoomScale="102" zoomScaleNormal="50" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1751,21 +1776,21 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="35">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="47">
         <v>45692</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="39">
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="51">
         <v>45934</v>
       </c>
-      <c r="K1" s="40"/>
+      <c r="K1" s="52"/>
       <c r="L1" s="27">
         <v>45692</v>
       </c>
@@ -2049,20 +2074,20 @@
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="47">
         <v>45965</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="42" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -2427,19 +2452,19 @@
         <v>76</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="43" t="s">
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="45"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="44"/>
       <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -2583,11 +2608,11 @@
         <v>81</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="46" t="s">
+      <c r="D25" s="46"/>
+      <c r="E25" s="35" t="s">
         <v>275</v>
       </c>
       <c r="F25" s="1"/>
@@ -2606,20 +2631,23 @@
       <c r="D26" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="E26" s="49" t="s">
+      <c r="E26" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="F26" s="49" t="s">
+      <c r="F26" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="36" t="s">
         <v>296</v>
       </c>
-      <c r="H26" s="52" t="s">
+      <c r="H26" s="39" t="s">
         <v>306</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>316</v>
+      </c>
+      <c r="K26" s="30" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2633,16 +2661,16 @@
       <c r="D27" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="E27" s="50" t="s">
+      <c r="E27" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="F27" s="50" t="s">
+      <c r="F27" s="37" t="s">
         <v>287</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="37" t="s">
         <v>298</v>
       </c>
-      <c r="H27" s="53" t="s">
+      <c r="H27" s="40" t="s">
         <v>307</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2660,16 +2688,16 @@
       <c r="D28" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="E28" s="50" t="s">
+      <c r="E28" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="F28" s="50" t="s">
+      <c r="F28" s="37" t="s">
         <v>288</v>
       </c>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="H28" s="53" t="s">
+      <c r="H28" s="40" t="s">
         <v>308</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2687,16 +2715,16 @@
       <c r="D29" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="E29" s="50" t="s">
+      <c r="E29" s="37" t="s">
         <v>279</v>
       </c>
-      <c r="F29" s="50" t="s">
+      <c r="F29" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="G29" s="37" t="s">
         <v>300</v>
       </c>
-      <c r="H29" s="53" t="s">
+      <c r="H29" s="40" t="s">
         <v>309</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2714,16 +2742,16 @@
       <c r="D30" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="E30" s="50" t="s">
+      <c r="E30" s="37" t="s">
         <v>280</v>
       </c>
-      <c r="F30" s="50" t="s">
+      <c r="F30" s="37" t="s">
         <v>290</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="37" t="s">
         <v>297</v>
       </c>
-      <c r="H30" s="53" t="s">
+      <c r="H30" s="40" t="s">
         <v>310</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2741,16 +2769,16 @@
       <c r="D31" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E31" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="F31" s="50" t="s">
+      <c r="F31" s="37" t="s">
         <v>291</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G31" s="37" t="s">
         <v>301</v>
       </c>
-      <c r="H31" s="53" t="s">
+      <c r="H31" s="40" t="s">
         <v>311</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2768,16 +2796,16 @@
       <c r="D32" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="E32" s="50" t="s">
+      <c r="E32" s="37" t="s">
         <v>282</v>
       </c>
-      <c r="F32" s="50" t="s">
+      <c r="F32" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="G32" s="50" t="s">
+      <c r="G32" s="37" t="s">
         <v>302</v>
       </c>
-      <c r="H32" s="53" t="s">
+      <c r="H32" s="40" t="s">
         <v>312</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -2795,19 +2823,21 @@
       <c r="D33" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="E33" s="50" t="s">
+      <c r="E33" s="37" t="s">
         <v>283</v>
       </c>
-      <c r="F33" s="50" t="s">
+      <c r="F33" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="G33" s="50" t="s">
+      <c r="G33" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="H33" s="53" t="s">
+      <c r="H33" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="I33" s="1"/>
+      <c r="I33" s="55" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -2820,19 +2850,21 @@
       <c r="D34" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="E34" s="50" t="s">
+      <c r="E34" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="F34" s="50" t="s">
+      <c r="F34" s="37" t="s">
         <v>294</v>
       </c>
-      <c r="G34" s="50" t="s">
+      <c r="G34" s="37" t="s">
         <v>304</v>
       </c>
-      <c r="H34" s="53" t="s">
+      <c r="H34" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="I34" s="1"/>
+      <c r="I34" s="55" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
@@ -2845,19 +2877,21 @@
       <c r="D35" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="38" t="s">
         <v>285</v>
       </c>
-      <c r="F35" s="51" t="s">
+      <c r="F35" s="38" t="s">
         <v>295</v>
       </c>
-      <c r="G35" s="51" t="s">
+      <c r="G35" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="H35" s="54" t="s">
+      <c r="H35" s="41" t="s">
         <v>315</v>
       </c>
-      <c r="I35" s="1"/>
+      <c r="I35" s="55" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="36" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
@@ -2869,7 +2903,9 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="I36" s="55" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
@@ -2881,7 +2917,9 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="I37" s="55" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -2893,7 +2931,9 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="I38" s="55" t="s">
+        <v>328</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2909,4 +2949,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95490B59-7F7F-4EEF-BC73-3B20B540C1EB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update CSV and Excel files for SMILES enumeration; add trail.py for SMILES processing
</commit_message>
<xml_diff>
--- a/Used_SMILES.xlsx
+++ b/Used_SMILES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B684897-BC69-42FC-9451-8611E335E259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66291B0-9A6C-433A-8A96-1D89A5B034BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Leemol" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="347">
   <si>
     <t>Till Now</t>
   </si>
@@ -1025,6 +1025,57 @@
   </si>
   <si>
     <t>M635</t>
+  </si>
+  <si>
+    <t>M566</t>
+  </si>
+  <si>
+    <t>M769</t>
+  </si>
+  <si>
+    <t>M1980</t>
+  </si>
+  <si>
+    <t>Leemol</t>
+  </si>
+  <si>
+    <t>30/04/2025</t>
+  </si>
+  <si>
+    <t>Christina Ma'am</t>
+  </si>
+  <si>
+    <t>M2860</t>
+  </si>
+  <si>
+    <t>M2859</t>
+  </si>
+  <si>
+    <t>M2812</t>
+  </si>
+  <si>
+    <t>M2858</t>
+  </si>
+  <si>
+    <t>M2841</t>
+  </si>
+  <si>
+    <t>M2811</t>
+  </si>
+  <si>
+    <t>M1055</t>
+  </si>
+  <si>
+    <t>M1174</t>
+  </si>
+  <si>
+    <t>M1202</t>
+  </si>
+  <si>
+    <t>M1214</t>
+  </si>
+  <si>
+    <t>M1249</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1091,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1059,44 +1110,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1262,11 +1277,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1277,12 +1301,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1292,54 +1310,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1348,49 +1321,10 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1430,7 +1364,77 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1747,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE12E00B-2345-41BD-89EE-DDF317AEFD3A}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F18" zoomScale="102" zoomScaleNormal="50" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="50" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1767,868 +1771,879 @@
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="24.77734375" customWidth="1"/>
     <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="47">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="17">
         <v>45692</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="51">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="21">
         <v>45934</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="27">
+      <c r="K1" s="22"/>
+      <c r="L1" s="10">
         <v>45692</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="5" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="39" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="26" t="s">
         <v>95</v>
       </c>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="40" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="26" t="s">
         <v>96</v>
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="26" t="s">
         <v>97</v>
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="26" t="s">
         <v>98</v>
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="26" t="s">
         <v>99</v>
       </c>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="26" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="17">
         <v>45965</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="26" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="26" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="26" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="32" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="L14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="L15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="L16" s="26"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="L17" s="26"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L17" s="9"/>
+      <c r="M17" s="41"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="L18" s="26"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="L19" s="26"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="42" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="42" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="26"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I22" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="K22" s="30" t="s">
+      <c r="K22" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="L22" s="26"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="I23" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="J23" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="K23" s="30" t="s">
+      <c r="K23" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="L23" s="26"/>
-    </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="H24" s="31" t="s">
+      <c r="H24" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="J24" s="31" t="s">
+      <c r="J24" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="K24" s="32" t="s">
+      <c r="K24" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="L24" s="26"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="D25" s="46"/>
-      <c r="E25" s="35" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="11" t="s">
         <v>275</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="42" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="35" t="s">
         <v>265</v>
       </c>
       <c r="E26" s="36" t="s">
@@ -2640,241 +2655,280 @@
       <c r="G26" s="36" t="s">
         <v>296</v>
       </c>
-      <c r="H26" s="39" t="s">
+      <c r="H26" s="37" t="s">
         <v>306</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="K26" s="30" t="s">
+      <c r="J26" s="43" t="s">
+        <v>342</v>
+      </c>
+      <c r="K26" s="43" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="35" t="s">
         <v>277</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="G27" s="37" t="s">
+      <c r="G27" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="H27" s="40" t="s">
+      <c r="H27" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I27" s="35" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J27" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="35" t="s">
         <v>267</v>
       </c>
-      <c r="E28" s="37" t="s">
+      <c r="E28" s="35" t="s">
         <v>278</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="G28" s="37" t="s">
+      <c r="G28" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="H28" s="40" t="s">
+      <c r="H28" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="35" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J28" s="48" t="s">
+        <v>344</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E29" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="F29" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="35" t="s">
         <v>300</v>
       </c>
-      <c r="H29" s="40" t="s">
+      <c r="H29" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="35" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J29" s="48" t="s">
+        <v>345</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="33" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="35" t="s">
         <v>269</v>
       </c>
-      <c r="E30" s="37" t="s">
+      <c r="E30" s="35" t="s">
         <v>280</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="G30" s="37" t="s">
+      <c r="G30" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="H30" s="40" t="s">
+      <c r="H30" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="35" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J30" s="49" t="s">
+        <v>346</v>
+      </c>
+      <c r="K30" s="43" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="33" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G31" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="H31" s="40" t="s">
+      <c r="H31" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I31" s="35" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K31" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="33" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="35" t="s">
         <v>271</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="35" t="s">
         <v>282</v>
       </c>
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="35" t="s">
         <v>302</v>
       </c>
-      <c r="H32" s="40" t="s">
+      <c r="H32" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I32" s="38" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K32" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="33" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="35" t="s">
         <v>272</v>
       </c>
-      <c r="E33" s="37" t="s">
+      <c r="E33" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F33" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="G33" s="37" t="s">
+      <c r="G33" s="35" t="s">
         <v>303</v>
       </c>
-      <c r="H33" s="40" t="s">
+      <c r="H33" s="45" t="s">
         <v>313</v>
       </c>
-      <c r="I33" s="55" t="s">
+      <c r="I33" s="47" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K33" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="33" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" s="35" t="s">
         <v>263</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="E34" s="37" t="s">
+      <c r="E34" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="F34" s="37" t="s">
+      <c r="F34" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="G34" s="37" t="s">
+      <c r="G34" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="H34" s="40" t="s">
+      <c r="H34" s="45" t="s">
         <v>314</v>
       </c>
-      <c r="I34" s="55" t="s">
+      <c r="I34" s="48" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K34" s="7" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="34" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="38" t="s">
         <v>274</v>
       </c>
       <c r="E35" s="38" t="s">
@@ -2886,14 +2940,17 @@
       <c r="G35" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="H35" s="41" t="s">
+      <c r="H35" s="46" t="s">
         <v>315</v>
       </c>
-      <c r="I35" s="55" t="s">
+      <c r="I35" s="48" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="44" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>92</v>
       </c>
@@ -2903,11 +2960,11 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="55" t="s">
+      <c r="I36" s="48" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>93</v>
       </c>
@@ -2917,11 +2974,11 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="55" t="s">
+      <c r="I37" s="48" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>94</v>
       </c>
@@ -2931,10 +2988,11 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="55" t="s">
+      <c r="I38" s="49" t="s">
         <v>328</v>
       </c>
     </row>
+    <row r="39" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C20:G20"/>

</xml_diff>

<commit_message>
Remove outdated CSV file and add new Excel file for singlet fission compounds
</commit_message>
<xml_diff>
--- a/Used_SMILES.xlsx
+++ b/Used_SMILES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Computer\Meh!!!!!!!\workspace\VIT_LAB\SingletFission_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66291B0-9A6C-433A-8A96-1D89A5B034BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D7B58-22B7-497F-9C0D-404CDA9D92E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{33D9803C-9BA7-428F-8170-F50661F7BBBB}"/>
   </bookViews>
@@ -1290,7 +1290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1325,6 +1325,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1363,79 +1430,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1781,21 +1775,21 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="17">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="40">
         <v>45692</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="21">
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="44">
         <v>45934</v>
       </c>
-      <c r="K1" s="22"/>
+      <c r="K1" s="45"/>
       <c r="L1" s="10">
         <v>45692</v>
       </c>
@@ -1837,7 +1831,7 @@
       <c r="L2" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="14" t="s">
         <v>333</v>
       </c>
     </row>
@@ -1848,38 +1842,38 @@
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="13" t="s">
         <v>95</v>
       </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="26" t="s">
         <v>335</v>
       </c>
     </row>
@@ -1890,34 +1884,34 @@
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="L4" s="13" t="s">
         <v>96</v>
       </c>
       <c r="M4" s="1"/>
@@ -1929,34 +1923,34 @@
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="13" t="s">
         <v>97</v>
       </c>
       <c r="M5" s="1"/>
@@ -1968,34 +1962,34 @@
       <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="K6" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="13" t="s">
         <v>98</v>
       </c>
       <c r="M6" s="1"/>
@@ -2007,34 +2001,34 @@
       <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="13" t="s">
         <v>99</v>
       </c>
       <c r="M7" s="1"/>
@@ -2046,34 +2040,34 @@
       <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="L8" s="13" t="s">
         <v>100</v>
       </c>
       <c r="M8" s="1"/>
@@ -2085,20 +2079,20 @@
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="40">
         <v>45965</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24" t="s">
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -2107,34 +2101,34 @@
       <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="L10" s="13" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2145,34 +2139,34 @@
       <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="L11" s="26" t="s">
+      <c r="L11" s="13" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2183,34 +2177,34 @@
       <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L12" s="26" t="s">
+      <c r="L12" s="13" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2221,34 +2215,34 @@
       <c r="B13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="L13" s="32" t="s">
+      <c r="L13" s="19" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2259,31 +2253,31 @@
       <c r="B14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="13" t="s">
         <v>210</v>
       </c>
       <c r="L14" s="9"/>
@@ -2293,31 +2287,31 @@
         <v>71</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="H15" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="I15" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="13" t="s">
         <v>211</v>
       </c>
       <c r="L15" s="9"/>
@@ -2327,31 +2321,31 @@
         <v>72</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="13" t="s">
         <v>214</v>
       </c>
       <c r="L16" s="9"/>
@@ -2361,66 +2355,66 @@
         <v>73</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="I17" s="26" t="s">
+      <c r="I17" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="13" t="s">
         <v>215</v>
       </c>
       <c r="L17" s="9"/>
-      <c r="M17" s="41"/>
+      <c r="M17" s="27"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="26" t="s">
+      <c r="H18" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="I18" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="13" t="s">
         <v>216</v>
       </c>
       <c r="L18" s="9"/>
@@ -2430,31 +2424,31 @@
         <v>75</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="K19" s="32" t="s">
+      <c r="K19" s="19" t="s">
         <v>217</v>
       </c>
       <c r="L19" s="9"/>
@@ -2464,19 +2458,19 @@
         <v>76</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="12" t="s">
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -2484,31 +2478,31 @@
         <v>77</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="I21" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="K21" s="12" t="s">
         <v>255</v>
       </c>
       <c r="L21" s="9"/>
@@ -2518,31 +2512,31 @@
         <v>78</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="H22" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="I22" s="26" t="s">
+      <c r="I22" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="K22" s="25" t="s">
+      <c r="K22" s="12" t="s">
         <v>256</v>
       </c>
       <c r="L22" s="9"/>
@@ -2552,31 +2546,31 @@
         <v>79</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="I23" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="K23" s="25" t="s">
+      <c r="K23" s="12" t="s">
         <v>257</v>
       </c>
       <c r="L23" s="9"/>
@@ -2586,31 +2580,31 @@
         <v>80</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="H24" s="32" t="s">
+      <c r="H24" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="I24" s="32" t="s">
+      <c r="I24" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="K24" s="33" t="s">
+      <c r="K24" s="20" t="s">
         <v>258</v>
       </c>
       <c r="L24" s="9"/>
@@ -2620,10 +2614,10 @@
         <v>81</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="D25" s="16"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="11" t="s">
         <v>275</v>
       </c>
@@ -2631,7 +2625,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="K25" s="42" t="s">
+      <c r="K25" s="28" t="s">
         <v>334</v>
       </c>
     </row>
@@ -2640,31 +2634,31 @@
         <v>82</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="F26" s="36" t="s">
+      <c r="F26" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="H26" s="37" t="s">
+      <c r="H26" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="J26" s="43" t="s">
+      <c r="J26" s="29" t="s">
         <v>342</v>
       </c>
-      <c r="K26" s="43" t="s">
+      <c r="K26" s="29" t="s">
         <v>329</v>
       </c>
     </row>
@@ -2673,25 +2667,25 @@
         <v>83</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="G27" s="35" t="s">
+      <c r="G27" s="22" t="s">
         <v>298</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="I27" s="35" t="s">
+      <c r="I27" s="22" t="s">
         <v>317</v>
       </c>
       <c r="J27" s="7" t="s">
@@ -2706,28 +2700,28 @@
         <v>84</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="G28" s="35" t="s">
+      <c r="G28" s="22" t="s">
         <v>299</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="I28" s="35" t="s">
+      <c r="I28" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="J28" s="48" t="s">
+      <c r="J28" s="33" t="s">
         <v>344</v>
       </c>
       <c r="K28" s="7" t="s">
@@ -2739,28 +2733,28 @@
         <v>85</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="G29" s="35" t="s">
+      <c r="G29" s="22" t="s">
         <v>300</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="I29" s="35" t="s">
+      <c r="I29" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="J29" s="48" t="s">
+      <c r="J29" s="33" t="s">
         <v>345</v>
       </c>
       <c r="K29" s="7" t="s">
@@ -2772,31 +2766,31 @@
         <v>86</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="G30" s="22" t="s">
         <v>297</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="I30" s="35" t="s">
+      <c r="I30" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="J30" s="49" t="s">
+      <c r="J30" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="K30" s="43" t="s">
+      <c r="K30" s="29" t="s">
         <v>336</v>
       </c>
     </row>
@@ -2805,25 +2799,25 @@
         <v>87</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="G31" s="35" t="s">
+      <c r="G31" s="22" t="s">
         <v>301</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I31" s="35" t="s">
+      <c r="I31" s="22" t="s">
         <v>321</v>
       </c>
       <c r="K31" s="7" t="s">
@@ -2835,25 +2829,25 @@
         <v>88</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="22" t="s">
         <v>302</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="I32" s="38" t="s">
+      <c r="I32" s="25" t="s">
         <v>322</v>
       </c>
       <c r="K32" s="7" t="s">
@@ -2865,25 +2859,25 @@
         <v>89</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="F33" s="35" t="s">
+      <c r="F33" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="H33" s="45" t="s">
+      <c r="H33" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="I33" s="47" t="s">
+      <c r="I33" s="32" t="s">
         <v>323</v>
       </c>
       <c r="K33" s="7" t="s">
@@ -2895,25 +2889,25 @@
         <v>90</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="G34" s="35" t="s">
+      <c r="G34" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="H34" s="45" t="s">
+      <c r="H34" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="I34" s="48" t="s">
+      <c r="I34" s="33" t="s">
         <v>325</v>
       </c>
       <c r="K34" s="7" t="s">
@@ -2925,28 +2919,28 @@
         <v>91</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="25" t="s">
         <v>274</v>
       </c>
-      <c r="E35" s="38" t="s">
+      <c r="E35" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="F35" s="38" t="s">
+      <c r="F35" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="G35" s="38" t="s">
+      <c r="G35" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="H35" s="46" t="s">
+      <c r="H35" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="I35" s="48" t="s">
+      <c r="I35" s="33" t="s">
         <v>324</v>
       </c>
-      <c r="K35" s="44" t="s">
+      <c r="K35" s="30" t="s">
         <v>341</v>
       </c>
     </row>
@@ -2960,7 +2954,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="48" t="s">
+      <c r="I36" s="33" t="s">
         <v>326</v>
       </c>
     </row>
@@ -2974,7 +2968,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="48" t="s">
+      <c r="I37" s="33" t="s">
         <v>327</v>
       </c>
     </row>
@@ -2988,7 +2982,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="49" t="s">
+      <c r="I38" s="34" t="s">
         <v>328</v>
       </c>
     </row>

</xml_diff>